<commit_message>
Update Projektplan with Phases and To Do´s
</commit_message>
<xml_diff>
--- a/Documentation/project-plan.xlsx
+++ b/Documentation/project-plan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanji\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanji\Documents\GitHub\Karteikarten-System\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{760553FA-C280-43B8-AC9B-E195F056D86B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D655F11D-A84F-4226-B36F-3C57B21079CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="99">
   <si>
     <t>Idea Planner</t>
   </si>
@@ -52,38 +52,15 @@
     <t>Topic:</t>
   </si>
   <si>
-    <t>Technology</t>
-  </si>
-  <si>
-    <t>Keywords:</t>
-  </si>
-  <si>
-    <t>Innovative, fresh, elegant</t>
-  </si>
-  <si>
-    <t>Plan Due Date:</t>
-  </si>
-  <si>
     <t>Name:</t>
   </si>
   <si>
-    <t>Team Dev</t>
-  </si>
-  <si>
     <t>Goal:</t>
   </si>
   <si>
     <t>Objective:</t>
   </si>
   <si>
-    <t xml:space="preserve">To win a grant or scholarships and a trip to Silicon Valley and Seattle.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Develop a technology solution for submission to the upcoming innovative app competition.
-</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Task Status Indicator</t>
   </si>
   <si>
@@ -99,31 +76,271 @@
     <t>Status Icon</t>
   </si>
   <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>Review competition rules</t>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Egor, Sanjivan</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Project Due Date:</t>
+  </si>
+  <si>
+    <t>Productivity-Game</t>
+  </si>
+  <si>
+    <t>Ziel der Anwendung schriftlich festhalten</t>
+  </si>
+  <si>
+    <t>Features auflisten (CRUD)</t>
+  </si>
+  <si>
+    <t>Wichtige Use-Cases beschreiben </t>
+  </si>
+  <si>
+    <t>Seiten festlegen</t>
+  </si>
+  <si>
+    <t>Zwecks- und Funktionsdefinition</t>
+  </si>
+  <si>
+    <t>Benutzerabläufe festlegen</t>
+  </si>
+  <si>
+    <t>Mockup</t>
+  </si>
+  <si>
+    <t>Farben, Typographie und Abstände definieren</t>
+  </si>
+  <si>
+    <t>UI-Komponenten ausarbeiten</t>
+  </si>
+  <si>
+    <t>Einheitliches Design festlegen</t>
+  </si>
+  <si>
+    <t>Mockup exportieren und ablegen</t>
+  </si>
+  <si>
+    <t>Entitäten festlegen</t>
+  </si>
+  <si>
+    <t>attribute, datentypen, PK festlegen</t>
+  </si>
+  <si>
+    <t>Beziehungen definieren</t>
+  </si>
+  <si>
+    <t>Kardinalitäten bestimmen</t>
+  </si>
+  <si>
+    <t>ER Diagramm erstellen</t>
+  </si>
+  <si>
+    <t>Relationales Diagramm erstellen</t>
+  </si>
+  <si>
+    <t>Diagramme ablegen</t>
+  </si>
+  <si>
+    <t>SQLite Scripte erstellen (Create, Insert, Programmability)</t>
+  </si>
+  <si>
+    <t>Ordnerstruktur für Services, Datenzugriff erstellen</t>
+  </si>
+  <si>
+    <t>Fehlerbehandlung für Datenbankzugriffe integrieren</t>
+  </si>
+  <si>
+    <t>Benutzer anlegen</t>
+  </si>
+  <si>
+    <t>Benutzer eindeutig identifizieren</t>
+  </si>
+  <si>
+    <t>Login-Logik implementieren</t>
+  </si>
+  <si>
+    <t>Validierung von Benutzereingaben</t>
+  </si>
+  <si>
+    <t>CRUD-Funktionalität für Tasks implementieren</t>
+  </si>
+  <si>
+    <t>Vue Projekt erstellen</t>
+  </si>
+  <si>
+    <t>Grundlayout umsetzen (Navbar, Footer)</t>
+  </si>
+  <si>
+    <t>Routing/ Navigation zwischen Seiten implementieren</t>
+  </si>
+  <si>
+    <t>Einheitliche UI/UX Elemente und Styles definieren</t>
+  </si>
+  <si>
+    <t>5.2 Task UI</t>
+  </si>
+  <si>
+    <t>Task Liste anzeigen</t>
+  </si>
+  <si>
+    <t>Task erstellen Formular (Titel, Schwierigkeit, Dauer, Kategorie)</t>
+  </si>
+  <si>
+    <t>Task bearbeiten / löschen</t>
+  </si>
+  <si>
+    <t>Task als erledigt markieren</t>
+  </si>
+  <si>
+    <t>Validierung implementieren (Feedback vom backend)</t>
+  </si>
+  <si>
+    <t>UI aktualisieren nach DB änderung (Refresh/Reload)</t>
+  </si>
+  <si>
+    <t>5.3 Gamification UI</t>
+  </si>
+  <si>
+    <t>XP anzeigen</t>
+  </si>
+  <si>
+    <t>Level anzeigen</t>
+  </si>
+  <si>
+    <t>Streak anzeigen</t>
+  </si>
+  <si>
+    <t>Nach erledigter Task Feedback zurückgeben</t>
+  </si>
+  <si>
+    <t>Phase 1: Planung &amp; Vorbereitung                        1.1: Projektdefinition</t>
+  </si>
+  <si>
+    <t>1.2: Feature-Liste &amp; Use-Cases</t>
+  </si>
+  <si>
+    <t>1.3: Datenanalyse &amp; Modellierung</t>
+  </si>
+  <si>
+    <t>Phase 2: UX/UI &amp; Struktur                                        2.1: Seitenstruktur</t>
+  </si>
+  <si>
+    <t>2.3: Mockup-Erstellung</t>
+  </si>
+  <si>
+    <t>3.2: Authentifizierung</t>
+  </si>
+  <si>
+    <t>Phase 3: Backend/DB - Basis                                   3.1: Grundsetup</t>
+  </si>
+  <si>
+    <t>Phase 5: Frontend – Kernfunktionen                  5.1: Grundlayout</t>
+  </si>
+  <si>
+    <t>Phase 8: Qualität und Abschluss                            8.1 Testing</t>
+  </si>
+  <si>
+    <t>Unit-Tests für zentrale Logik</t>
+  </si>
+  <si>
+    <t>Tests für Datenbankzugriffe</t>
+  </si>
+  <si>
+    <t>Testfälle mit gültigen und ungültigen Eingaben</t>
+  </si>
+  <si>
+    <t>Fehlerbehandlung gezielt prüfen</t>
+  </si>
+  <si>
+    <t>8.2 Finalisierung</t>
+  </si>
+  <si>
+    <t>Bugs beheben</t>
+  </si>
+  <si>
+    <t>Code verbessern (Lesbarkeit/ Struktur)</t>
+  </si>
+  <si>
+    <t>Kommentare / Best Practise</t>
+  </si>
+  <si>
+    <t>Projekt testen (lokal)</t>
+  </si>
+  <si>
+    <t>8.3 Release</t>
+  </si>
+  <si>
+    <t>Github Actions vorbereiten</t>
+  </si>
+  <si>
+    <t>Projekt veröffentlichen</t>
   </si>
   <si>
     <t>Yes</t>
   </si>
   <si>
-    <t>Add links to project resources here</t>
-  </si>
-  <si>
-    <t>Research prior winning technologies</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Develop &amp; test app</t>
+    <t>Webapplikation, Produktivität, Gamification</t>
+  </si>
+  <si>
+    <t>Responsibility</t>
+  </si>
+  <si>
+    <t>Sanjivan</t>
+  </si>
+  <si>
+    <t>Projektplan bestimmen</t>
+  </si>
+  <si>
+    <t>Egor</t>
+  </si>
+  <si>
+    <t>Sanjivan &amp; Egor</t>
+  </si>
+  <si>
+    <t>Navigation bestimmen</t>
+  </si>
+  <si>
+    <t>Create Scipt schreiben</t>
+  </si>
+  <si>
+    <t>Insert Script schreiben</t>
+  </si>
+  <si>
+    <t>Programmability Script schreiben</t>
+  </si>
+  <si>
+    <t>Beim Projekt handelt es sich um eine Web basierte Anwendung, welche die Produktivität des Benutzers fördern soll. Dies wird mit einem Spielerischem Ansatz erreicht (Gamification). Die Website soll Nutzern ermöglichen Tasks zu verwalten und abzuarbeiten, gleichzeitig aber den Nutzern zu motivieren die Task zu erledigen. Dafür werden Elemente der Spielebranche benutzt wie XP, Level, Streaks, welche die Arbeit messbar macht und motivierend wirkt.</t>
+  </si>
+  <si>
+    <t>Projekt builden</t>
   </si>
   <si>
     <t>Pending</t>
   </si>
   <si>
-    <t>Write documentation</t>
+    <t>Projektauftrag beschreiben</t>
+  </si>
+  <si>
+    <t>SMART Ziele bestimmen</t>
+  </si>
+  <si>
+    <t>1.4: Backend-Design</t>
+  </si>
+  <si>
+    <t>Methoden definieren passend zur DB</t>
+  </si>
+  <si>
+    <t>Backend-Projekt in JS erstellen</t>
+  </si>
+  <si>
+    <t>SQL als lokale Datenbank anbinden</t>
+  </si>
+  <si>
+    <t>3.3: Karteikarten-Logik</t>
+  </si>
+  <si>
+    <t>Dokumentation prüfen auf Vollständigkeit</t>
   </si>
 </sst>
 </file>
@@ -233,7 +450,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -255,6 +472,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="-0.24994659260841701"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -347,7 +576,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -360,9 +589,6 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="15" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="9" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="3" fillId="3" borderId="3" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -377,6 +603,75 @@
     </xf>
     <xf numFmtId="168" fontId="12" fillId="4" borderId="0" xfId="19" applyFill="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="12" fillId="4" borderId="0" xfId="19">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="18" applyFont="1" applyFill="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="9" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="18" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="9" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="12" fillId="5" borderId="0" xfId="19" applyFill="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="5" borderId="0" xfId="18" applyFont="1" applyFill="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="9" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="9" fillId="5" borderId="0" xfId="19" applyFont="1" applyFill="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="0" xfId="18" applyFont="1" applyFill="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="9" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="12" fillId="6" borderId="0" xfId="19" applyFill="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="9" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="12" fillId="4" borderId="0" xfId="19" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="18" applyFont="1" applyFill="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="9" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -413,7 +708,7 @@
     <cellStyle name="Währung" xfId="12" builtinId="4" customBuiltin="1"/>
     <cellStyle name="Währung [0]" xfId="13" builtinId="7" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="11">
     <dxf>
       <font>
         <color theme="5" tint="-0.499984740745262"/>
@@ -433,6 +728,29 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="8" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="&quot;Complete&quot;;&quot;Incomplete or Overdue&quot;;&quot;Pending or Due Tomorrow&quot;"/>
     </dxf>
     <dxf>
       <border>
@@ -492,10 +810,10 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="Idea Planner" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Idea Planner" pivot="0" count="4" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="6"/>
-      <tableStyleElement type="headerRow" dxfId="5"/>
-      <tableStyleElement type="firstColumn" dxfId="4"/>
-      <tableStyleElement type="firstHeaderCell" dxfId="3"/>
+      <tableStyleElement type="wholeTable" dxfId="10"/>
+      <tableStyleElement type="headerRow" dxfId="9"/>
+      <tableStyleElement type="firstColumn" dxfId="8"/>
+      <tableStyleElement type="firstHeaderCell" dxfId="7"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -522,7 +840,7 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>295275</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>114</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -564,13 +882,9 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tasks" displayName="Tasks" ref="B6:G10" totalsRowShown="0">
-  <autoFilter ref="B6:G10" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tasks" displayName="Tasks" ref="B6:G83" totalsRowShown="0">
+  <autoFilter ref="B6:G83" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -588,7 +902,9 @@
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Status Icon" dataCellStyle="Status Icon Text">
       <calculatedColumnFormula>IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Notes"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Responsibility" dataDxfId="6">
+      <calculatedColumnFormula>IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="Idea Planner" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -866,188 +1182,1704 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:G10"/>
+  <dimension ref="B1:G83"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:G4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A63" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="1" max="1" width="2.5546875" customWidth="1"/>
     <col min="2" max="2" width="1" customWidth="1"/>
-    <col min="3" max="3" width="43.33203125" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" customWidth="1"/>
+    <col min="3" max="3" width="42.5546875" customWidth="1"/>
+    <col min="4" max="4" width="18.5546875" customWidth="1"/>
     <col min="5" max="5" width="22.5546875" customWidth="1"/>
     <col min="6" max="6" width="31" customWidth="1"/>
-    <col min="7" max="7" width="43.33203125" customWidth="1"/>
-    <col min="8" max="8" width="2.6640625" customWidth="1"/>
+    <col min="7" max="7" width="43.44140625" customWidth="1"/>
+    <col min="8" max="8" width="2.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
     </row>
     <row r="2" spans="2:7" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="11"/>
+      <c r="C2" s="33"/>
       <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="2:7" ht="33" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="4">
+        <v>46185</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G3" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" ht="28.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="2:7" ht="33" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="5">
-        <f ca="1">TODAY()</f>
-        <v>46058</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" ht="28.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
     </row>
     <row r="5" spans="2:7" ht="75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
+      <c r="B5" s="35" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
     </row>
     <row r="6" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="7" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" s="14"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="16" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G7" s="25"/>
+    </row>
+    <row r="8" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="7">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="D8" s="6">
+        <v>46080</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F8" s="8">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>1</v>
+      </c>
+      <c r="G8" s="26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="10">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D9" s="6">
+        <v>46080</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F9" s="8">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>0</v>
+      </c>
+      <c r="G9" s="26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="7">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>92</v>
+      </c>
+      <c r="D10" s="6">
+        <v>46080</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="8">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G10" s="26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="10">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>81</v>
+      </c>
+      <c r="D11" s="6">
+        <v>46080</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F11" s="8">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>0</v>
+      </c>
+      <c r="G11" s="26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="10" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="18"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="20" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G12" s="27"/>
+    </row>
+    <row r="13" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="10">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C13" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="D13" s="11">
+        <v>46079</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="10">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G13" s="26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="10">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C14" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="D14" s="11">
+        <v>46079</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="10">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G14" s="26" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="10" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" s="22"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="24" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G15" s="28"/>
+    </row>
+    <row r="16" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="10">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="11">
+        <v>46086</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="10">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G16" s="26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="10">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="11">
+        <v>46086</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="10">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G17" s="26" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="10">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="11">
+        <v>46086</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="10">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G18" s="26" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="10">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="11">
+        <v>46086</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="10">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G19" s="26" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="10">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" s="11">
+        <v>46086</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="10">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G20" s="26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="10">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="11">
+        <v>46086</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" s="10">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G21" s="26" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="10">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" s="11">
+        <v>46086</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" s="10">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G22" s="26" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="10" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="C23" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="D23" s="22"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="24" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G23" s="24"/>
+    </row>
+    <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="10">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C24" t="s">
+        <v>94</v>
+      </c>
+      <c r="D24" s="11">
+        <v>46093</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" s="10">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G24" s="29" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="10" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D25" s="30"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="16" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G25" s="16"/>
+    </row>
+    <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="10">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C26" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="8">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v>1</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="D26" s="11">
+        <v>46100</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" s="10">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="10">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C27" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="7">
-        <f ca="1">PlanDueDate-15</f>
-        <v>46043</v>
-      </c>
-      <c r="E7" s="4" t="s">
+      <c r="D27" s="11">
+        <v>46100</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" s="10">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="10">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C28" t="s">
+        <v>84</v>
+      </c>
+      <c r="D28" s="11">
+        <v>46100</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F28" s="10">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G28" s="10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="10">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C29" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="9">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v>1</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="D29" s="11">
+        <v>46100</v>
+      </c>
+      <c r="E29" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" s="10">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G29" s="10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="10" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D30" s="30"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="16" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G30" s="25"/>
+    </row>
+    <row r="31" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="10">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D31" s="11">
+        <v>46107</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F31" s="10">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G31" s="26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="10">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C32" t="s">
+        <v>22</v>
+      </c>
+      <c r="D32" s="11">
+        <v>46107</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F32" s="10">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G32" s="26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="10">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C33" t="s">
+        <v>23</v>
+      </c>
+      <c r="D33" s="11">
+        <v>46107</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F33" s="10">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G33" s="26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="10">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C34" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="8">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v>-1</v>
-      </c>
-      <c r="C8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="7">
-        <f ca="1">PlanDueDate-12</f>
-        <v>46046</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" s="9">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="8">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v>0</v>
-      </c>
-      <c r="C9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="7">
-        <f ca="1">PlanDueDate-10</f>
-        <v>46048</v>
-      </c>
-      <c r="E9" s="4" t="s">
+      <c r="D34" s="11">
+        <v>46112</v>
+      </c>
+      <c r="E34" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F34" s="10">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G34" s="26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="10">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C35" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="9">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="8">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v>-1</v>
-      </c>
-      <c r="C10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="7">
-        <f ca="1">PlanDueDate-5</f>
-        <v>46053</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" s="9">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v>-1</v>
+      <c r="D35" s="11">
+        <v>46112</v>
+      </c>
+      <c r="E35" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F35" s="10">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G35" s="26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="10" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="C36" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="D36" s="22"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="24" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G36" s="28"/>
+    </row>
+    <row r="37" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="10">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C37" t="s">
+        <v>32</v>
+      </c>
+      <c r="D37" s="11">
+        <v>46107</v>
+      </c>
+      <c r="E37" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F37" s="10">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G37" s="26" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="10">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C38" t="s">
+        <v>85</v>
+      </c>
+      <c r="D38" s="11">
+        <v>46107</v>
+      </c>
+      <c r="E38" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F38" s="10">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G38" s="26" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="10">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C39" t="s">
+        <v>86</v>
+      </c>
+      <c r="D39" s="11">
+        <v>46112</v>
+      </c>
+      <c r="E39" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F39" s="10">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G39" s="26" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="10">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C40" t="s">
+        <v>87</v>
+      </c>
+      <c r="D40" s="11">
+        <v>46112</v>
+      </c>
+      <c r="E40" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F40" s="10">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G40" s="26" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="10">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C41" t="s">
+        <v>33</v>
+      </c>
+      <c r="D41" s="11">
+        <v>46135</v>
+      </c>
+      <c r="E41" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F41" s="10">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G41" s="26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="10">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C42" t="s">
+        <v>95</v>
+      </c>
+      <c r="D42" s="11">
+        <v>46135</v>
+      </c>
+      <c r="E42" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F42" s="10">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G42" s="26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="10">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C43" t="s">
+        <v>96</v>
+      </c>
+      <c r="D43" s="11">
+        <v>46135</v>
+      </c>
+      <c r="E43" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F43" s="10">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G43" s="26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="10">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C44" t="s">
+        <v>34</v>
+      </c>
+      <c r="D44" s="11">
+        <v>46111</v>
+      </c>
+      <c r="E44" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F44" s="10">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G44" s="26" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="10" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="C45" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D45" s="22"/>
+      <c r="E45" s="23"/>
+      <c r="F45" s="24" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G45" s="28"/>
+    </row>
+    <row r="46" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="10">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C46" t="s">
+        <v>35</v>
+      </c>
+      <c r="D46" s="11">
+        <v>46111</v>
+      </c>
+      <c r="E46" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F46" s="10">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G46" s="26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="10">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C47" t="s">
+        <v>36</v>
+      </c>
+      <c r="D47" s="11">
+        <v>46111</v>
+      </c>
+      <c r="E47" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F47" s="10">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G47" s="26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="10">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C48" t="s">
+        <v>37</v>
+      </c>
+      <c r="D48" s="11">
+        <v>46111</v>
+      </c>
+      <c r="E48" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F48" s="10">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G48" s="26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="10">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C49" t="s">
+        <v>38</v>
+      </c>
+      <c r="D49" s="11">
+        <v>46111</v>
+      </c>
+      <c r="E49" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F49" s="10">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G49" s="26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="10" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="C50" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="D50" s="22"/>
+      <c r="E50" s="23"/>
+      <c r="F50" s="24" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G50" s="28"/>
+    </row>
+    <row r="51" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B51" s="10">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C51" t="s">
+        <v>39</v>
+      </c>
+      <c r="D51" s="11">
+        <v>46111</v>
+      </c>
+      <c r="E51" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F51" s="10">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G51" s="26" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="10" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="C52" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="D52" s="22"/>
+      <c r="E52" s="23"/>
+      <c r="F52" s="24" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G52" s="28"/>
+    </row>
+    <row r="53" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="10">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C53" t="s">
+        <v>40</v>
+      </c>
+      <c r="D53" s="11">
+        <v>46116</v>
+      </c>
+      <c r="E53" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F53" s="10">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G53" s="26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="10">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C54" t="s">
+        <v>41</v>
+      </c>
+      <c r="D54" s="11">
+        <v>46116</v>
+      </c>
+      <c r="E54" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F54" s="10">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G54" s="26" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="55" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B55" s="10">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C55" t="s">
+        <v>42</v>
+      </c>
+      <c r="D55" s="11">
+        <v>46116</v>
+      </c>
+      <c r="E55" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F55" s="10">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G55" s="26" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="10">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C56" t="s">
+        <v>43</v>
+      </c>
+      <c r="D56" s="11">
+        <v>46116</v>
+      </c>
+      <c r="E56" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F56" s="10">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G56" s="26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B57" s="10" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="C57" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="D57" s="22"/>
+      <c r="E57" s="23"/>
+      <c r="F57" s="24" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G57" s="28"/>
+    </row>
+    <row r="58" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="10">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C58" t="s">
+        <v>45</v>
+      </c>
+      <c r="D58" s="11">
+        <v>46117</v>
+      </c>
+      <c r="E58" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F58" s="10">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G58" s="26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="59" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="10">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C59" t="s">
+        <v>46</v>
+      </c>
+      <c r="D59" s="11">
+        <v>46119</v>
+      </c>
+      <c r="E59" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F59" s="10">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G59" s="26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="60" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B60" s="10">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C60" t="s">
+        <v>47</v>
+      </c>
+      <c r="D60" s="11">
+        <v>46119</v>
+      </c>
+      <c r="E60" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F60" s="10">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G60" s="26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="61" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B61" s="10">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C61" t="s">
+        <v>48</v>
+      </c>
+      <c r="D61" s="11">
+        <v>46119</v>
+      </c>
+      <c r="E61" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F61" s="10">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G61" s="26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="62" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B62" s="10">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C62" t="s">
+        <v>49</v>
+      </c>
+      <c r="D62" s="11">
+        <v>46120</v>
+      </c>
+      <c r="E62" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F62" s="10">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G62" s="26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="63" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B63" s="10">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C63" t="s">
+        <v>50</v>
+      </c>
+      <c r="D63" s="11">
+        <v>46120</v>
+      </c>
+      <c r="E63" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F63" s="10">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G63" s="26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="64" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B64" s="10" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="C64" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="D64" s="22"/>
+      <c r="E64" s="23"/>
+      <c r="F64" s="24" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G64" s="28"/>
+    </row>
+    <row r="65" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B65" s="10">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C65" t="s">
+        <v>52</v>
+      </c>
+      <c r="D65" s="11">
+        <v>46123</v>
+      </c>
+      <c r="E65" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F65" s="10">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G65" s="26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="66" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B66" s="10">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C66" t="s">
+        <v>53</v>
+      </c>
+      <c r="D66" s="11">
+        <v>46123</v>
+      </c>
+      <c r="E66" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F66" s="10">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G66" s="26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="67" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B67" s="10">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C67" t="s">
+        <v>54</v>
+      </c>
+      <c r="D67" s="11">
+        <v>46123</v>
+      </c>
+      <c r="E67" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F67" s="10">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G67" s="26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="68" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B68" s="10">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C68" t="s">
+        <v>55</v>
+      </c>
+      <c r="D68" s="11">
+        <v>46123</v>
+      </c>
+      <c r="E68" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F68" s="10">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G68" s="26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="69" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B69" s="10" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="C69" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="D69" s="22"/>
+      <c r="E69" s="23"/>
+      <c r="F69" s="24" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G69" s="28"/>
+    </row>
+    <row r="70" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B70" s="10">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C70" t="s">
+        <v>65</v>
+      </c>
+      <c r="D70" s="11">
+        <v>46163</v>
+      </c>
+      <c r="E70" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F70" s="10">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G70" s="26" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="71" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B71" s="10">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C71" t="s">
+        <v>66</v>
+      </c>
+      <c r="D71" s="11">
+        <v>46170</v>
+      </c>
+      <c r="E71" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F71" s="10">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G71" s="26" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="72" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B72" s="10">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C72" t="s">
+        <v>67</v>
+      </c>
+      <c r="D72" s="11">
+        <v>46170</v>
+      </c>
+      <c r="E72" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F72" s="10">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G72" s="26" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="73" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B73" s="10">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C73" t="s">
+        <v>68</v>
+      </c>
+      <c r="D73" s="11">
+        <v>46170</v>
+      </c>
+      <c r="E73" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F73" s="10">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G73" s="26" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="74" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B74" s="10" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="C74" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="D74" s="22"/>
+      <c r="E74" s="23"/>
+      <c r="F74" s="24" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G74" s="28"/>
+    </row>
+    <row r="75" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B75" s="10">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C75" t="s">
+        <v>70</v>
+      </c>
+      <c r="D75" s="11">
+        <v>46177</v>
+      </c>
+      <c r="E75" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F75" s="10">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G75" s="26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="76" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B76" s="10">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C76" t="s">
+        <v>71</v>
+      </c>
+      <c r="D76" s="11">
+        <v>46177</v>
+      </c>
+      <c r="E76" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F76" s="10">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G76" s="26" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="77" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B77" s="10">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C77" t="s">
+        <v>72</v>
+      </c>
+      <c r="D77" s="11">
+        <v>46177</v>
+      </c>
+      <c r="E77" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F77" s="10">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G77" s="26" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="78" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B78" s="10">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C78" t="s">
+        <v>98</v>
+      </c>
+      <c r="D78" s="11">
+        <v>46177</v>
+      </c>
+      <c r="E78" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F78" s="10">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G78" s="26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="79" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B79" s="10">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C79" t="s">
+        <v>73</v>
+      </c>
+      <c r="D79" s="11">
+        <v>46177</v>
+      </c>
+      <c r="E79" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F79" s="10">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G79" s="26" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="80" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B80" s="10" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="C80" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="D80" s="22"/>
+      <c r="E80" s="23"/>
+      <c r="F80" s="24" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G80" s="28"/>
+    </row>
+    <row r="81" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B81" s="10">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C81" t="s">
+        <v>75</v>
+      </c>
+      <c r="D81" s="11">
+        <v>46185</v>
+      </c>
+      <c r="E81" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F81" s="10">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G81" s="26" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="82" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B82" s="10">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C82" t="s">
+        <v>89</v>
+      </c>
+      <c r="D82" s="11">
+        <v>46185</v>
+      </c>
+      <c r="E82" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F82" s="10">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G82" s="26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="83" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B83" s="10">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C83" t="s">
+        <v>76</v>
+      </c>
+      <c r="D83" s="11">
+        <v>46185</v>
+      </c>
+      <c r="E83" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F83" s="10">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G83" s="26" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1059,8 +2891,8 @@
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="B5:D5"/>
   </mergeCells>
-  <conditionalFormatting sqref="B7:B10">
-    <cfRule type="colorScale" priority="17">
+  <conditionalFormatting sqref="B7:B83">
+    <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="num" val="-1"/>
         <cfvo type="num" val="0"/>
@@ -1071,17 +2903,17 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F7:F10">
-    <cfRule type="expression" dxfId="2" priority="1">
-      <formula>F7=1</formula>
+  <conditionalFormatting sqref="G23:G29">
+    <cfRule type="expression" dxfId="5" priority="57">
+      <formula>G23=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="2">
-      <formula>F7=0</formula>
+    <cfRule type="expression" dxfId="4" priority="58">
+      <formula>G23=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="3">
-      <formula>F7=-1</formula>
+    <cfRule type="expression" dxfId="3" priority="59">
+      <formula>G23=-1</formula>
     </cfRule>
-    <cfRule type="iconSet" priority="18">
+    <cfRule type="iconSet" priority="60">
       <iconSet iconSet="3Symbols2">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="0"/>
@@ -1089,29 +2921,47 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations xWindow="198" yWindow="610" count="22">
+  <conditionalFormatting sqref="F7:F83">
+    <cfRule type="expression" dxfId="2" priority="101">
+      <formula>F7=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="102">
+      <formula>F7=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="103">
+      <formula>F7=-1</formula>
+    </cfRule>
+    <cfRule type="iconSet" priority="104">
+      <iconSet iconSet="3Symbols2">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations disablePrompts="1" xWindow="1660" yWindow="543" count="20">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Create an Idea Planner in this worksheet. Set a Goal and an Objective, and enter task details in the Tasks table" sqref="A1" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Image is in this cell. Title of this worksheet is in cell below" sqref="B1" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Topic in cell at right" sqref="D2" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Topic in this cell" sqref="E2" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Keywords in cell at right" sqref="F2" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Keywords in this cell" sqref="G2" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Plan Due Date in cell at right" sqref="D3" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Plan Due Date in this cell" sqref="E3" xr:uid="{00000000-0002-0000-0000-000007000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Name in cell at right" sqref="F3" xr:uid="{00000000-0002-0000-0000-000008000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Name in this cell" sqref="G3" xr:uid="{00000000-0002-0000-0000-000009000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Goal in cell below" sqref="B4:D4" xr:uid="{00000000-0002-0000-0000-00000A000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Objective in cell below" sqref="E4:G4" xr:uid="{00000000-0002-0000-0000-00000B000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Objective in cell below" sqref="E4:F4" xr:uid="{00000000-0002-0000-0000-00000B000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Goal in this cell" sqref="B5:D5" xr:uid="{00000000-0002-0000-0000-00000C000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This column is automatically updated and indicates status based on column F" sqref="B6" xr:uid="{00000000-0002-0000-0000-00000D000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Tasks in this column under this heading" sqref="C6" xr:uid="{00000000-0002-0000-0000-00000E000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Due Date in this column under this heading" sqref="D6" xr:uid="{00000000-0002-0000-0000-00000F000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Notes in this column under this heading" sqref="G6" xr:uid="{00000000-0002-0000-0000-000010000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select task completion status in this column. Press ALT+DOWN ARROW to open the drop-down list, ENTER to make selection. An icon representing this status is in the column at right" sqref="E6" xr:uid="{00000000-0002-0000-0000-000011000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Status icons in this column are automatically updated based on Done column value &amp; comparing Due Dates. Dates beyond the due date &amp; just before the due date are noted for emphasis" sqref="F6" xr:uid="{00000000-0002-0000-0000-000012000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Objective in this cell" sqref="E5:G5" xr:uid="{00000000-0002-0000-0000-000013000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Objective in this cell" sqref="E5:F5" xr:uid="{00000000-0002-0000-0000-000013000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of this worksheet is in this cell. Enter idea details in cells at right. Enter Goal and Objective below. Enter tasks in Tasks table below" sqref="B2:C3" xr:uid="{00000000-0002-0000-0000-000014000000}"/>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select an option from the list. Press Cancel then ALT+DOWN ARROW to open the drop-down list, then ENTER to make selection" sqref="E7:E10" xr:uid="{00000000-0002-0000-0000-000015000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576" xr:uid="{482F76EC-3095-4ECD-80A0-E3C86F6A9FD3}">
+      <formula1>"Sanjivan,Egor,Sanjivan &amp; Egor, Unbestimmt"</formula1>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select an option from the list. Press Cancel then ALT+DOWN ARROW to open the drop-down list, then ENTER to make selection" sqref="E7:E83" xr:uid="{00000000-0002-0000-0000-000015000000}">
       <formula1>"Yes, No, Pending"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>